<commit_message>
added secured password + refactoring
</commit_message>
<xml_diff>
--- a/RPA Project/OLXDataScrapingResults.xlsx
+++ b/RPA Project/OLXDataScrapingResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LA FACULTATEEEE\An III, sem 1\RPA\RPA-Project-JE03\RPA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B991107-CDE6-4A5D-A4BF-731875ED7A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A1654C-64DE-4178-9514-C2CB9FBE5286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -52,151 +52,145 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Audi A6 Audi A6 Avant 3.0 TDI quattro, An model 2017, Istoric service complet</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/audi-a6-avant-ID7GQidn.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>19 899,18 €</t>
-  </si>
-  <si>
-    <t>Floresti</t>
-  </si>
-  <si>
-    <t>Azi 14:00</t>
-  </si>
-  <si>
-    <t>Vând Audi A6 2.0 TDI</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/vand-audi-a6-2-0-tdi-IDe34a0.html#67f979e89d;promoted</t>
-  </si>
-  <si>
-    <t>12 999 €</t>
-  </si>
-  <si>
-    <t>Campina</t>
-  </si>
-  <si>
-    <t>Azi 13:46</t>
-  </si>
-  <si>
-    <t>Vand/schimb audi a6 3.0 tdi</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/vand-schimb-audi-a6-3-0-tdi-IDfFrfc.html#67f979e89d;promoted</t>
-  </si>
-  <si>
-    <t>2 800 €</t>
-  </si>
-  <si>
-    <t>Constanta</t>
-  </si>
-  <si>
-    <t>Azi 13:36</t>
-  </si>
-  <si>
-    <t>AUDI A6 2.7 Tdi*180cp* 2006* IMPECABIL!!!</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/audi-a6-2-7-tdi180cp-2006-impecabil-IDfv42P.html#67f979e89d;promoted</t>
-  </si>
-  <si>
-    <t>3 850 €</t>
-  </si>
-  <si>
-    <t>Botosani</t>
-  </si>
-  <si>
-    <t>Azi 13:32</t>
-  </si>
-  <si>
-    <t>Audi a6 4.2 v8 300 cp quattro</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/audi-a6-4-2-v8-300-cp-quattro-IDfFr9V.html#67f979e89d</t>
-  </si>
-  <si>
-    <t>4 200 €</t>
+    <t>Honda Civic Prim proprietar / carte service și istoric verificabil la Honda</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/honda-civic-1-5-ID7GWuaF.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>20 000 €</t>
+  </si>
+  <si>
+    <t>Cumpana</t>
+  </si>
+  <si>
+    <t>Azi 20:37</t>
+  </si>
+  <si>
+    <t>Honda civic model 2</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/honda-civic-model-2-IDfFwpn.html#4e6472c1f5</t>
+  </si>
+  <si>
+    <t>4 900 €</t>
   </si>
   <si>
     <t>Targoviste</t>
   </si>
   <si>
-    <t>Azi 13:29</t>
-  </si>
-  <si>
-    <t>Audi A6 Audi A6 40 TDI Avant , 204 cp, leasing avans 15%</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/audi-a6-avant-ID7GWq4E.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>39 865 €</t>
-  </si>
-  <si>
-    <t>Bucuresti, Sectorul 3</t>
-  </si>
-  <si>
-    <t>Azi 13:24</t>
-  </si>
-  <si>
-    <t>Audi A6 C7 3.0TDI Quattro</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/audi-a6-c7-3-0tdi-quattro-IDfAyAA.html#67f979e89d</t>
-  </si>
-  <si>
-    <t>12 850 €</t>
-  </si>
-  <si>
-    <t>Negresti-Oas</t>
-  </si>
-  <si>
-    <t>Audi A6 C6 3.0 tdi</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/audi-a6-c6-3-0-tdi-IDfFr5X.html#67f979e89d</t>
-  </si>
-  <si>
-    <t>6 200 €</t>
-  </si>
-  <si>
-    <t>Craiova</t>
-  </si>
-  <si>
-    <t>Azi 13:23</t>
-  </si>
-  <si>
-    <t>Audi A6</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/audi-a6-ID7GTFf5.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>46 900 €</t>
-  </si>
-  <si>
-    <t>Bucuresti, Sectorul 1</t>
-  </si>
-  <si>
-    <t>Azi 13:16</t>
-  </si>
-  <si>
-    <t>Audi A6 2.7 Quattro</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/audi-a6-2-7-quattro-IDfvL4r.html#67f979e89d;promoted</t>
-  </si>
-  <si>
-    <t>5 400 €</t>
-  </si>
-  <si>
-    <t>Fagaras</t>
-  </si>
-  <si>
-    <t>Azi 13:08</t>
+    <t>Azi 20:14</t>
+  </si>
+  <si>
+    <t>Honda Civic EJ9 1997</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/honda-civic-ej9-1997-IDfA6RK.html#4e6472c1f5</t>
+  </si>
+  <si>
+    <t>1 700 €</t>
+  </si>
+  <si>
+    <t>Satu Mare</t>
+  </si>
+  <si>
+    <t>Azi 19:23</t>
+  </si>
+  <si>
+    <t>Honda Civic</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/honda-civic-ID7GwjVG.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>8 050 €</t>
+  </si>
+  <si>
+    <t>Timisoara</t>
+  </si>
+  <si>
+    <t>Azi 19:00</t>
+  </si>
+  <si>
+    <t>Honda civic 2010 full, volan dreapta 2.2 diesel</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/honda-civic-2010-full-volan-dreapta-2-2-diesel-IDfFu0Q.html#4e6472c1f5</t>
+  </si>
+  <si>
+    <t>1 900 €</t>
+  </si>
+  <si>
+    <t>Onesti</t>
+  </si>
+  <si>
+    <t>Azi 17:42</t>
+  </si>
+  <si>
+    <t>Vand Honda Civic</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-honda-civic-IDfBia5.html#4e6472c1f5;promoted</t>
+  </si>
+  <si>
+    <t>3 650 €</t>
+  </si>
+  <si>
+    <t>Azi 16:51</t>
+  </si>
+  <si>
+    <t>Honda Civic honda civic Civic 1.5 Sport Plus LED#PANO#SPUR#KEYLESS#SHZ</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/honda-civic-ID7GWu5Z.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>26 990,39 €</t>
+  </si>
+  <si>
+    <t>Otopeni</t>
+  </si>
+  <si>
+    <t>Azi 16:34</t>
+  </si>
+  <si>
+    <t>Honda Civic honda civic Civic Limousine 1.5 Executive Automatik *Leder*</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/honda-civic-ID7GWu5U.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>18 990,02 €</t>
+  </si>
+  <si>
+    <t>Honda Civic Facelift 5DR 1.8 I-VTEC 140CP Euro 5 134k km</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/honda-civic-facelift-5dr-1-8-i-vtec-140cp-euro-5-134k-km-IDfBhGG.html#4e6472c1f5;promoted</t>
+  </si>
+  <si>
+    <t>6 250 €</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>Azi 16:13</t>
+  </si>
+  <si>
+    <t>Honda Civic ej2 America coupe inmatriculată</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/honda-civic-ej2-america-coupe-inmatriculata-IDfbh5u.html#4e6472c1f5;promoted</t>
+  </si>
+  <si>
+    <t>3 250 €</t>
+  </si>
+  <si>
+    <t>Pantelimon</t>
+  </si>
+  <si>
+    <t>Azi 15:44</t>
   </si>
 </sst>
 </file>
@@ -547,7 +541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2649479D-9E10-46D7-91AD-8EC075171E74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BC116B-6D8A-4D18-B649-90E92444AC3E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -667,27 +661,27 @@
         <v>32</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -701,44 +695,44 @@
         <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrated full flow + implemented dynamic selectors for filtrations
</commit_message>
<xml_diff>
--- a/RPA Project/OLXDataScrapingResults.xlsx
+++ b/RPA Project/OLXDataScrapingResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LA FACULTATEEEE\An III, sem 1\RPA\RPA-Project-JE03\RPA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A1654C-64DE-4178-9514-C2CB9FBE5286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D88860-0FDF-4ED0-97EF-F27057234F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -52,145 +52,139 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Honda Civic Prim proprietar / carte service și istoric verificabil la Honda</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/honda-civic-1-5-ID7GWuaF.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>20 000 €</t>
-  </si>
-  <si>
-    <t>Cumpana</t>
-  </si>
-  <si>
-    <t>Azi 20:37</t>
-  </si>
-  <si>
-    <t>Honda civic model 2</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/honda-civic-model-2-IDfFwpn.html#4e6472c1f5</t>
-  </si>
-  <si>
-    <t>4 900 €</t>
-  </si>
-  <si>
-    <t>Targoviste</t>
-  </si>
-  <si>
-    <t>Azi 20:14</t>
-  </si>
-  <si>
-    <t>Honda Civic EJ9 1997</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/honda-civic-ej9-1997-IDfA6RK.html#4e6472c1f5</t>
-  </si>
-  <si>
-    <t>1 700 €</t>
-  </si>
-  <si>
-    <t>Satu Mare</t>
-  </si>
-  <si>
-    <t>Azi 19:23</t>
-  </si>
-  <si>
-    <t>Honda Civic</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/honda-civic-ID7GwjVG.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>8 050 €</t>
+    <t>Brasov</t>
+  </si>
+  <si>
+    <t>Azi 22:16</t>
+  </si>
+  <si>
+    <t>Opel Corsa D 1.2</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-d-1-2-IDfyj8M.html#714b7e881f;promoted</t>
+  </si>
+  <si>
+    <t>2 700 €</t>
   </si>
   <si>
     <t>Timisoara</t>
   </si>
   <si>
-    <t>Azi 19:00</t>
-  </si>
-  <si>
-    <t>Honda civic 2010 full, volan dreapta 2.2 diesel</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/honda-civic-2010-full-volan-dreapta-2-2-diesel-IDfFu0Q.html#4e6472c1f5</t>
-  </si>
-  <si>
-    <t>1 900 €</t>
-  </si>
-  <si>
-    <t>Onesti</t>
-  </si>
-  <si>
-    <t>Azi 17:42</t>
-  </si>
-  <si>
-    <t>Vand Honda Civic</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/vand-honda-civic-IDfBia5.html#4e6472c1f5;promoted</t>
-  </si>
-  <si>
-    <t>3 650 €</t>
-  </si>
-  <si>
-    <t>Azi 16:51</t>
-  </si>
-  <si>
-    <t>Honda Civic honda civic Civic 1.5 Sport Plus LED#PANO#SPUR#KEYLESS#SHZ</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/honda-civic-ID7GWu5Z.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>26 990,39 €</t>
-  </si>
-  <si>
-    <t>Otopeni</t>
-  </si>
-  <si>
-    <t>Azi 16:34</t>
-  </si>
-  <si>
-    <t>Honda Civic honda civic Civic Limousine 1.5 Executive Automatik *Leder*</t>
-  </si>
-  <si>
-    <t>https://www.autovit.ro/anunt/honda-civic-ID7GWu5U.html#xtor=SEC-81</t>
-  </si>
-  <si>
-    <t>18 990,02 €</t>
-  </si>
-  <si>
-    <t>Honda Civic Facelift 5DR 1.8 I-VTEC 140CP Euro 5 134k km</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/honda-civic-facelift-5dr-1-8-i-vtec-140cp-euro-5-134k-km-IDfBhGG.html#4e6472c1f5;promoted</t>
-  </si>
-  <si>
-    <t>6 250 €</t>
-  </si>
-  <si>
-    <t>Cluj-Napoca</t>
-  </si>
-  <si>
-    <t>Azi 16:13</t>
-  </si>
-  <si>
-    <t>Honda Civic ej2 America coupe inmatriculată</t>
-  </si>
-  <si>
-    <t>https://www.olx.ro/d/oferta/honda-civic-ej2-america-coupe-inmatriculata-IDfbh5u.html#4e6472c1f5;promoted</t>
-  </si>
-  <si>
-    <t>3 250 €</t>
-  </si>
-  <si>
-    <t>Pantelimon</t>
-  </si>
-  <si>
-    <t>Azi 15:44</t>
+    <t>Azi 22:52</t>
+  </si>
+  <si>
+    <t>Opel Corsa AUTOMATA Benzina 1.2 Climatronic RATE</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/opel-corsa-1-2-ID7GWly1.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>3 990 €</t>
+  </si>
+  <si>
+    <t>Bacau</t>
+  </si>
+  <si>
+    <t>Opel Corsa 1,2 benzina Automata</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-1-2-benzina-automata-IDfvuA0.html#714b7e881f;promoted</t>
+  </si>
+  <si>
+    <t>2 790 €</t>
+  </si>
+  <si>
+    <t>Ghirdoveni</t>
+  </si>
+  <si>
+    <t>Azi 21:58</t>
+  </si>
+  <si>
+    <t>Opel Corsa 2004 / 1.0 benzina / 60cp / Stare generala buna/recent adus</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-2004-1-0-benzina-60cp-stare-generala-buna-recent-adus-IDfDuhE.html#714b7e881f;promoted</t>
+  </si>
+  <si>
+    <t>1 299 €</t>
+  </si>
+  <si>
+    <t>Ganeasa</t>
+  </si>
+  <si>
+    <t>Azi 21:27</t>
+  </si>
+  <si>
+    <t>Opel Corsa 2009/1.4 Benzina/Posibilitate Plata RATE</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-2009-1-4-benzina-posibilitate-plata-rate-IDfEZGA.html#714b7e881f;promoted</t>
+  </si>
+  <si>
+    <t>3 299 €</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Azi 21:14</t>
+  </si>
+  <si>
+    <t>Opel Corsa 2007 Automata Benzina RATE</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/opel-corsa-1-2i-ID7GL1Mr.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>Azi 21:03</t>
+  </si>
+  <si>
+    <t>Opel corsa 1.2 benzina</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-1-2-benzina-IDfrI9M.html#714b7e881f;promoted</t>
+  </si>
+  <si>
+    <t>2 800 €</t>
+  </si>
+  <si>
+    <t>Buzau</t>
+  </si>
+  <si>
+    <t>Azi 20:45</t>
+  </si>
+  <si>
+    <t>Vand Opel Corsa C</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-opel-corsa-c-IDfFFaV.html#714b7e881f</t>
+  </si>
+  <si>
+    <t>Vaslui</t>
+  </si>
+  <si>
+    <t>Azi 20:35</t>
+  </si>
+  <si>
+    <t>Opel Corsa 2011 AUTOMATA Euro 5 Rate</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/opel-corsa-ID7GJECP.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>5 850 €</t>
+  </si>
+  <si>
+    <t>Azi 20:24</t>
+  </si>
+  <si>
+    <t>Opel corsa D 1.3 90cp</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/opel-corsa-d-1-3-90cp-IDfFF42.html#714b7e881f</t>
+  </si>
+  <si>
+    <t>1 750 €</t>
   </si>
 </sst>
 </file>
@@ -567,101 +561,101 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -691,28 +685,28 @@
       <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>707</v>
+      </c>
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -729,10 +723,10 @@
         <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a new filtration for location refactoring clean code
</commit_message>
<xml_diff>
--- a/RPA Project/OLXDataScrapingResults.xlsx
+++ b/RPA Project/OLXDataScrapingResults.xlsx
@@ -1,41 +1,276 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LA FACULTATEEEE\An III, sem 1\RPA\RPA-Project-JE03\RPA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AB32D1-A8F7-4E3D-B274-0AB7C01A081A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedData" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>* Audi A4 2009 S-Line E5 * Bi-Xenon / Alcantara / Led / Navi Mare *</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-2009-s-line-e5-bi-xenon-alcantara-led-navi-mare-IDfEXdt.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>6 990 €</t>
+  </si>
+  <si>
+    <t>Oradea</t>
+  </si>
+  <si>
+    <t>Azi 16:31</t>
+  </si>
+  <si>
+    <t>Audi A4 Sline 2014, 2.0 TDI quattro</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-sline-2014-2-0-tdi-quattro-IDfA7QF.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>12 750 €</t>
+  </si>
+  <si>
+    <t>Azi 15:23</t>
+  </si>
+  <si>
+    <t>Vand Audi A4 b8 an 2013</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-audi-a4-b8-an-2013-IDfGVb9.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>1 821 €</t>
+  </si>
+  <si>
+    <t>Azi 14:59</t>
+  </si>
+  <si>
+    <t>Vand Audi A4 b8 2013 pret 9.200 euro negociabil</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-audi-a4-b8-2013-pret-9-200-euro-negociabil-IDfBMmZ.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>Azi 14:53</t>
+  </si>
+  <si>
+    <t>Vând sau schimb Audi A4 b9 2016 2.0 tdi 150 cp</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-sau-schimb-audi-a4-b9-2016-2-0-tdi-150-cp-IDfvwY6.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>12 499 €</t>
+  </si>
+  <si>
+    <t>Azi 13:20</t>
+  </si>
+  <si>
+    <t>A4 model 2009</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/a4-model-2009-IDfGTdN.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>6 200 €</t>
+  </si>
+  <si>
+    <t>Azi 11:44</t>
+  </si>
+  <si>
+    <t>Audi A4 model 2009</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-model-2009-IDfGT9b.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>Azi 11:39</t>
+  </si>
+  <si>
+    <t>Audi A4 2.0tdi an 2011 full</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-2-0tdi-an-2011-full-IDfGLWO.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>7 150 €</t>
+  </si>
+  <si>
+    <t>Azi 08:43</t>
+  </si>
+  <si>
+    <t>Audi A4 B7 2.0 TFSI Quattro Automat + GPL</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-b7-2-0-tfsi-quattro-automat-gpl-IDfGQfB.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>5 299 €</t>
+  </si>
+  <si>
+    <t>Azi 00:04</t>
+  </si>
+  <si>
+    <t>Audi A 4 impecabil</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a-4-impecabil-IDfGQ1t.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>5 995 €</t>
+  </si>
+  <si>
+    <t>Ieri 23:28</t>
+  </si>
+  <si>
+    <t>Vând Audi A4/ B8 /2010/97000 km/Euro 5</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-audi-a4-b8-2010-97000-km-euro-5-IDduVlE.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>9 990 €</t>
+  </si>
+  <si>
+    <t>Ieri 21:29</t>
+  </si>
+  <si>
+    <t>Audi A4 1.8 TFSI 170 CP - automat</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-1-8-tfsi-170-cp-automat-IDfGOC4.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>10 290 €</t>
+  </si>
+  <si>
+    <t>Ieri 21:15</t>
+  </si>
+  <si>
+    <t>Audi A4 AUDI A4,ACC,Front,Sighn,Lanne Assist,Camera,Matrixx Bi Xenon,Navi MMI+</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/audi-a4-avant-ID7GUqMS.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>16 390 €</t>
+  </si>
+  <si>
+    <t>Ieri 16:15</t>
+  </si>
+  <si>
+    <t>De vanzare Audi A4 2010</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/de-vanzare-audi-a4-2010-IDfhCYD.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>Ieri 14:47</t>
+  </si>
+  <si>
+    <t>Vând audi a4</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vand-audi-a4-IDerHbF.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>4 600 €</t>
+  </si>
+  <si>
+    <t>Ieri 14:18</t>
+  </si>
+  <si>
+    <t>Vînd audi a4 b7,1,9</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/vind-audi-a4-b7-1-9-IDe9le1.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>4 100 €</t>
+  </si>
+  <si>
+    <t>Ieri 13:29</t>
+  </si>
+  <si>
+    <t>Audi A4 Anul 2005 1.9 tdi 116cp Euro4 Xenon Incalzire Scaune Jante</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-anul-2005-1-9-tdi-116cp-euro4-xenon-incalzire-scaune-jante-IDfGzm3.html#fd993a50de</t>
+  </si>
+  <si>
+    <t>2 950 €</t>
+  </si>
+  <si>
+    <t>4 ian</t>
+  </si>
+  <si>
+    <t>Audi A4 2.0 TDI S-Line Euro 5 Xenon Navi Automat</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-2-0-tdi-s-line-euro-5-xenon-navi-automat-IDfq5rE.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>7 490 €</t>
+  </si>
+  <si>
+    <t>Audi A4 Audi A4 B8 an 2008</t>
+  </si>
+  <si>
+    <t>https://www.autovit.ro/anunt/audi-a4-2-7-ID7GOgrr.html#xtor=SEC-81</t>
+  </si>
+  <si>
+    <t>6 000 €</t>
+  </si>
+  <si>
+    <t>AUDI A4 B9 2016,</t>
+  </si>
+  <si>
+    <t>https://www.olx.ro/d/oferta/audi-a4-b9-2016-IDfzF1r.html#fd993a50de;promoted</t>
+  </si>
+  <si>
+    <t>20 999 €</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,8 +300,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,19 +616,385 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE168149-4771-4096-8A03-648D8D2228AC}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>